<commit_message>
Update Daily_Time_Series test cases.xlsx
</commit_message>
<xml_diff>
--- a/Daily_Time_Series test cases.xlsx
+++ b/Daily_Time_Series test cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gautam Tasvik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gautam Tasvik\Documents\Time_Series_Daily\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="1094">
   <si>
     <t>TestCase#</t>
   </si>
@@ -3270,14 +3270,73 @@
 https://www.alphavantage.co/query?function=TIME_SERIES_DAILY&amp;symbol=IBM&amp;apikey=demo&amp;datatype=csv</t>
   </si>
   <si>
+    <t>Verify test case 4 and 8 with optional datatype parameter</t>
+  </si>
+  <si>
+    <t>same as test case 4 and 8 appending datatype=csv to the get request</t>
+  </si>
+  <si>
+    <t>Meta Data</t>
+  </si>
+  <si>
+    <t>Verify symbol in the response meta data should be IBM</t>
+  </si>
+  <si>
     <t>1.Status code should be 200.
-2.Request should be in csv format</t>
-  </si>
-  <si>
-    <t>Verify test case 4 and 8 with optional datatype parameter</t>
-  </si>
-  <si>
-    <t>same as test case 4 and 8 appending datatype=csv to the get request</t>
+2.Response meta data symbol should show IBM.</t>
+  </si>
+  <si>
+    <t>1.Status code should be 200.
+2.Response should be in csv format</t>
+  </si>
+  <si>
+    <t>Verify symbol in the response meta data should be TSCO.LON</t>
+  </si>
+  <si>
+    <t>1.Status code should be 200.
+2.Response meta data symbol should show TSCO.LON.</t>
+  </si>
+  <si>
+    <t>Verify Output Size in the response meta data should be Full Size</t>
+  </si>
+  <si>
+    <t>1.Status code should be 200.
+2.Response meta data Output Size should show Full Size.</t>
+  </si>
+  <si>
+    <t>1.Send GET request to 
+https://www.alphavantage.co/query?function=TIME_SERIES_DAILY&amp;symbol=TSCO.LON&amp;apikey=demo</t>
+  </si>
+  <si>
+    <t>1.Status code should be 200.
+2.Response meta data Output Size should show Compact.</t>
+  </si>
+  <si>
+    <t>Verify Output Size in the response meta data should be Compact</t>
+  </si>
+  <si>
+    <t>Verify Time Zone in the response meta data should be US/Eastern</t>
+  </si>
+  <si>
+    <t>1.Status code should be 200.
+2.Response meta data Output Size should show US/Eastern.</t>
+  </si>
+  <si>
+    <t>API Response</t>
+  </si>
+  <si>
+    <t>Response should contain Meta Data and Time Series (Daily)</t>
+  </si>
+  <si>
+    <t>1.Status code should be 200.
+2.Response should contain Meta Data and Time Series (Daily).</t>
+  </si>
+  <si>
+    <t>Verify Information in the response meta data should be Daily Prices (open, high, low, close) and Volumes</t>
+  </si>
+  <si>
+    <t>1.Status code should be 200.
+2.Response meta data Information should show Daily Prices (open, high, low, close) and Volumes.</t>
   </si>
 </sst>
 </file>
@@ -3312,7 +3371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3335,11 +3394,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3352,6 +3424,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3634,10 +3712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3704,7 +3782,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="105">
+    <row r="4" spans="1:7" ht="75">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -3791,7 +3869,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="105">
+    <row r="9" spans="1:7" ht="75">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -3878,7 +3956,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="135">
+    <row r="14" spans="1:7" ht="120">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -3930,7 +4008,7 @@
         <v>1073</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>1074</v>
+        <v>1079</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -3940,19 +4018,152 @@
         <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>1074</v>
+        <v>1079</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1">
+      <c r="A18" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="75">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="75">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75">
+      <c r="A24" s="3">
+        <v>19</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="2" customFormat="1">
+      <c r="A25" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="75">
+      <c r="A26" s="3">
+        <v>19</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>1091</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>